<commit_message>
nay - Movie API, Screen Fix
</commit_message>
<xml_diff>
--- a/documentation/02_基本設計/02_設計書_機能画面API一覧.xlsx
+++ b/documentation/02_基本設計/02_設計書_機能画面API一覧.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\Java\class\Documentation\OJT Project\02_基本設計\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\Java\class\Eclipse\ojt-project\documentation\02_基本設計\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24042" windowHeight="9742"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24042" windowHeight="9742" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="機能画面一覧" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="103">
   <si>
     <t>機能画面一覧</t>
   </si>
@@ -380,6 +380,12 @@
   </si>
   <si>
     <t>ムービー作成（管理用）</t>
+  </si>
+  <si>
+    <t>/admin/movie/title/{title}</t>
+  </si>
+  <si>
+    <t>（管理用）同タイトルムービーチェック</t>
   </si>
 </sst>
 </file>
@@ -1044,11 +1050,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="112" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="112" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C28" sqref="C28"/>
+      <selection pane="bottomRight" activeCell="A15" sqref="A15:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.05"/>
@@ -1500,17 +1506,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="35.88671875" customWidth="1"/>
+    <col min="1" max="1" width="40.21875" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
     <col min="3" max="3" width="8.109375" customWidth="1"/>
     <col min="4" max="4" width="11.77734375" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" customWidth="1"/>
+    <col min="5" max="5" width="44.5546875" customWidth="1"/>
     <col min="6" max="6" width="14.77734375" customWidth="1"/>
     <col min="7" max="7" width="15.5546875" customWidth="1"/>
     <col min="8" max="9" width="14.77734375" bestFit="1" customWidth="1"/>
@@ -1874,18 +1882,18 @@
       <c r="I17" s="32"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="34" t="s">
-        <v>71</v>
+      <c r="A18" s="35" t="s">
+        <v>102</v>
       </c>
       <c r="B18" s="35" t="s">
-        <v>40</v>
+        <v>101</v>
       </c>
       <c r="C18" s="32" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="34"/>
       <c r="E18" s="34" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="F18" s="32"/>
       <c r="G18" s="32"/>
@@ -1894,17 +1902,15 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B19" s="35" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="34" t="s">
-        <v>59</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D19" s="34"/>
       <c r="E19" s="34" t="s">
         <v>74</v>
       </c>
@@ -1915,15 +1921,17 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="34" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B20" s="35" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="34"/>
+        <v>23</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>59</v>
+      </c>
       <c r="E20" s="34" t="s">
         <v>74</v>
       </c>
@@ -1934,17 +1942,17 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="34" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B21" s="35" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="C21" s="32" t="s">
         <v>21</v>
       </c>
       <c r="D21" s="34"/>
       <c r="E21" s="34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F21" s="32"/>
       <c r="G21" s="32"/>
@@ -1953,17 +1961,17 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="34" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B22" s="35" t="s">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="C22" s="32" t="s">
         <v>21</v>
       </c>
       <c r="D22" s="34"/>
       <c r="E22" s="34" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="F22" s="32"/>
       <c r="G22" s="32"/>
@@ -1972,28 +1980,47 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="34" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="B23" s="35" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="C23" s="32" t="s">
         <v>21</v>
       </c>
       <c r="D23" s="34"/>
       <c r="E23" s="34" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="F23" s="32"/>
       <c r="G23" s="32"/>
       <c r="H23" s="32"/>
       <c r="I23" s="32"/>
     </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I7"/>
   <phoneticPr fontId="7"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C21">
       <formula1>"GET,POST,PUT,DELETE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>